<commit_message>
update CEA input data
</commit_message>
<xml_diff>
--- a/data/raw/Cost-Effectiveness.xlsx
+++ b/data/raw/Cost-Effectiveness.xlsx
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,13 +663,13 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>3.3500000000000001E-3</v>
+        <v>3.2074999999999998E-3</v>
       </c>
       <c r="D3">
-        <v>8.0499999999999999E-3</v>
+        <v>8.7881000000000001E-3</v>
       </c>
       <c r="E3">
-        <v>515</v>
+        <v>523.63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -744,13 +744,13 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>1.0699999999999999E-2</v>
+        <v>1.4116999999999999E-2</v>
       </c>
       <c r="D12">
-        <v>3.6700000000000001E-3</v>
+        <v>5.0807999999999999E-3</v>
       </c>
       <c r="E12">
-        <v>210</v>
+        <v>250.76</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -761,13 +761,13 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>6.8500000000000002E-3</v>
+        <v>8.0391999999999998E-3</v>
       </c>
       <c r="D13">
-        <v>1.44E-2</v>
+        <v>1.7024999999999998E-2</v>
       </c>
       <c r="E13">
-        <v>3776</v>
+        <v>4270.7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -794,13 +794,13 @@
         <v>4</v>
       </c>
       <c r="C16">
-        <v>4.3499999999999997E-3</v>
+        <v>9.1035000000000005E-3</v>
       </c>
       <c r="D16">
-        <v>2.9099999999999998E-3</v>
+        <v>5.9988999999999997E-3</v>
       </c>
       <c r="E16">
-        <v>-46.5</v>
+        <v>-41.917999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -907,13 +907,13 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <v>1.8599999999999998E-2</v>
+        <v>3.3685E-2</v>
       </c>
       <c r="D29">
-        <v>1.66E-2</v>
+        <v>2.8514999999999999E-2</v>
       </c>
       <c r="E29">
-        <v>-79.400000000000006</v>
+        <v>-116.15</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,13 +1004,13 @@
         <v>4</v>
       </c>
       <c r="C40">
-        <v>-4.9199999999999999E-3</v>
+        <v>-3.1381E-3</v>
       </c>
       <c r="D40">
-        <v>-5.7000000000000002E-3</v>
+        <v>-7.0622000000000002E-3</v>
       </c>
       <c r="E40">
-        <v>-110</v>
+        <v>-88.346999999999994</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,13 +1029,13 @@
         <v>4</v>
       </c>
       <c r="C42">
-        <v>5.28E-3</v>
+        <v>6.6353000000000002E-3</v>
       </c>
       <c r="D42">
-        <v>3.3999999999999998E-3</v>
+        <v>4.3991999999999998E-3</v>
       </c>
       <c r="E42">
-        <v>384</v>
+        <v>414.74</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,13 +1070,13 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>2.3600000000000001E-3</v>
+        <v>3.8760000000000001E-3</v>
       </c>
       <c r="D46">
-        <v>2.5400000000000002E-3</v>
+        <v>3.6898999999999999E-3</v>
       </c>
       <c r="E46">
-        <v>614</v>
+        <v>701.41</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1159,13 +1159,13 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>1.95E-2</v>
+        <v>2.2783000000000001E-2</v>
       </c>
       <c r="D56">
-        <v>1.24E-2</v>
+        <v>1.4047E-2</v>
       </c>
       <c r="E56">
-        <v>560</v>
+        <v>568.11</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>